<commit_message>
ASKAPSDP-2214 Added UCD fields from CASDA specs
</commit_message>
<xml_diff>
--- a/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
+++ b/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Catalogue description" sheetId="2" r:id="rId1"/>
     <sheet name="Comparison with Selavy" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="H2" authorId="0" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="177">
   <si>
     <t>Column order</t>
   </si>
@@ -496,13 +496,103 @@
   </si>
   <si>
     <t>Including in the LSM view for testing, but it is not actually required</t>
+  </si>
+  <si>
+    <t>ucd</t>
+  </si>
+  <si>
+    <t>meta.id;meta.main</t>
+  </si>
+  <si>
+    <t>meta.id</t>
+  </si>
+  <si>
+    <t>pos.eq.ra</t>
+  </si>
+  <si>
+    <t>pos.eq.dec</t>
+  </si>
+  <si>
+    <t>pos.eq.ra;meta.main</t>
+  </si>
+  <si>
+    <t>pos.eq.dec;meta.main</t>
+  </si>
+  <si>
+    <t>stat.error;pos.eq.ra</t>
+  </si>
+  <si>
+    <t>stat.error;pos.eq.dec</t>
+  </si>
+  <si>
+    <t>em.freq</t>
+  </si>
+  <si>
+    <t>phot.flux.density;stat.max;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t>stat.error;phot.flux.density;stat.max;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t>phot.flux.density;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t>stat.error;phot.flux.density;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t>phys.angSize.smajAxis;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t>phys.angSize.sminAxis;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t>phys.angSize;pos.posAng;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t>stat.error;phys.angSize.smajAxis;em.radio</t>
+  </si>
+  <si>
+    <t>stat.error;phys.angSize.sminAxis;em.radio</t>
+  </si>
+  <si>
+    <t>stat.error;phys.angSize;pos.posAng;em.radio</t>
+  </si>
+  <si>
+    <t>phys.angSize.smajAxis;em.radio;askap:meta.deconvolved</t>
+  </si>
+  <si>
+    <t>phys.angSize.sminAxis;em.radio;askap:meta.deconvolved</t>
+  </si>
+  <si>
+    <t>phys.angSize;pos.posAng;em.radio;askap:meta.deconvolved</t>
+  </si>
+  <si>
+    <t>stat.fit.chi2</t>
+  </si>
+  <si>
+    <t>stat.stdev;stat.fit</t>
+  </si>
+  <si>
+    <t>spect.index;em.radio</t>
+  </si>
+  <si>
+    <t>askap:spect.curvature;em.radio</t>
+  </si>
+  <si>
+    <t>stat.stdev;phot.flux.density</t>
+  </si>
+  <si>
+    <t>meta.code</t>
+  </si>
+  <si>
+    <t>meta.note</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,13 +680,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -623,7 +725,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -639,8 +741,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -680,15 +783,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -704,38 +802,50 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="16">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -750,6 +860,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="15" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1079,1016 +1190,1120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="18" style="11" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="15" style="17" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="32" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="17"/>
-    <col min="8" max="8" width="10" style="17" customWidth="1"/>
-    <col min="9" max="9" width="61.85546875" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="12"/>
+    <col min="2" max="2" width="68.28515625" style="29" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="18" style="11" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="15" style="16" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="25" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="16"/>
+    <col min="9" max="9" width="10" style="16" customWidth="1"/>
+    <col min="10" max="10" width="61.85546875" style="11" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="42" customHeight="1">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:11" ht="42" customHeight="1">
+      <c r="A1" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="21"/>
-      <c r="F1" s="27"/>
-      <c r="I1" s="21"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="18"/>
+      <c r="G1" s="22"/>
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.95" customHeight="1">
+      <c r="A2" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="F2" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="H2" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="I2" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="26" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:11" s="32" customFormat="1" ht="15">
+      <c r="A3" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="31"/>
+      <c r="C3" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="D3" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="E3" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="E3" s="28">
-        <v>1</v>
-      </c>
-      <c r="F3" s="29">
-        <v>1</v>
-      </c>
-      <c r="G3" s="28">
-        <v>1</v>
-      </c>
-      <c r="H3" s="28">
-        <v>0</v>
-      </c>
-      <c r="I3" s="22"/>
-    </row>
-    <row r="4" spans="1:10" s="26" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="F3" s="23">
+        <v>1</v>
+      </c>
+      <c r="G3" s="23">
+        <v>1</v>
+      </c>
+      <c r="H3" s="23">
+        <v>1</v>
+      </c>
+      <c r="I3" s="23">
+        <v>0</v>
+      </c>
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="1:11" s="32" customFormat="1" ht="15">
+      <c r="A4" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="D4" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="28">
-        <v>1</v>
-      </c>
-      <c r="F4" s="29">
-        <v>1</v>
-      </c>
-      <c r="G4" s="28">
-        <v>0</v>
-      </c>
-      <c r="H4" s="28">
-        <v>1</v>
-      </c>
-      <c r="I4" s="22" t="s">
+      <c r="E4" s="19"/>
+      <c r="F4" s="23">
+        <v>1</v>
+      </c>
+      <c r="G4" s="23">
+        <v>1</v>
+      </c>
+      <c r="H4" s="23">
+        <v>0</v>
+      </c>
+      <c r="I4" s="23">
+        <v>1</v>
+      </c>
+      <c r="J4" s="19" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="15">
+      <c r="A5" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="D5" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="18">
-        <v>1</v>
-      </c>
-      <c r="F5" s="30">
-        <v>1</v>
-      </c>
-      <c r="G5" s="18">
-        <v>1</v>
-      </c>
-      <c r="H5" s="18">
-        <v>0</v>
-      </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="17"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A6" s="19" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="24">
+        <v>1</v>
+      </c>
+      <c r="G5" s="24">
+        <v>1</v>
+      </c>
+      <c r="H5" s="24">
+        <v>1</v>
+      </c>
+      <c r="I5" s="24">
+        <v>0</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="25"/>
+    </row>
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="15">
+      <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="18">
-        <v>1</v>
-      </c>
-      <c r="F6" s="30">
-        <v>0</v>
-      </c>
-      <c r="G6" s="18">
-        <v>1</v>
-      </c>
-      <c r="H6" s="18">
-        <v>0</v>
-      </c>
-      <c r="I6" s="22"/>
-      <c r="J6"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A7" s="19" t="s">
+      <c r="E6" s="14"/>
+      <c r="F6" s="24">
+        <v>1</v>
+      </c>
+      <c r="G6" s="24">
+        <v>0</v>
+      </c>
+      <c r="H6" s="24">
+        <v>1</v>
+      </c>
+      <c r="I6" s="24">
+        <v>0</v>
+      </c>
+      <c r="J6" s="19"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="15">
+      <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="D7" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="18">
-        <v>0</v>
-      </c>
-      <c r="F7" s="30">
-        <v>0</v>
-      </c>
-      <c r="G7" s="18">
-        <v>0</v>
-      </c>
-      <c r="H7" s="18">
-        <v>0</v>
-      </c>
-      <c r="I7" s="14" t="s">
+      <c r="E7" s="14"/>
+      <c r="F7" s="24">
+        <v>0</v>
+      </c>
+      <c r="G7" s="24">
+        <v>0</v>
+      </c>
+      <c r="H7" s="24">
+        <v>0</v>
+      </c>
+      <c r="I7" s="24">
+        <v>0</v>
+      </c>
+      <c r="J7" s="14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A8" s="19" t="s">
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="15">
+      <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="D8" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="E8" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="18">
-        <v>0</v>
-      </c>
-      <c r="F8" s="30">
-        <v>0</v>
-      </c>
-      <c r="G8" s="18">
-        <v>0</v>
-      </c>
-      <c r="H8" s="18">
-        <v>0</v>
-      </c>
-      <c r="I8" s="14" t="s">
+      <c r="F8" s="24">
+        <v>0</v>
+      </c>
+      <c r="G8" s="24">
+        <v>0</v>
+      </c>
+      <c r="H8" s="24">
+        <v>0</v>
+      </c>
+      <c r="I8" s="24">
+        <v>0</v>
+      </c>
+      <c r="J8" s="14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A9" s="19" t="s">
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="15">
+      <c r="A9" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="D9" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="E9" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="18">
-        <v>0</v>
-      </c>
-      <c r="F9" s="30">
-        <v>0</v>
-      </c>
-      <c r="G9" s="18">
-        <v>0</v>
-      </c>
-      <c r="H9" s="18">
-        <v>0</v>
-      </c>
-      <c r="I9" s="14" t="s">
+      <c r="F9" s="24">
+        <v>0</v>
+      </c>
+      <c r="G9" s="24">
+        <v>0</v>
+      </c>
+      <c r="H9" s="24">
+        <v>0</v>
+      </c>
+      <c r="I9" s="24">
+        <v>0</v>
+      </c>
+      <c r="J9" s="14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="15">
+      <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="D10" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="E10" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="18">
-        <v>1</v>
-      </c>
-      <c r="F10" s="30">
-        <v>0</v>
-      </c>
-      <c r="G10" s="18">
-        <v>0</v>
-      </c>
-      <c r="H10" s="18">
-        <v>1</v>
-      </c>
-      <c r="I10" s="23"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A11" s="19" t="s">
+      <c r="F10" s="24">
+        <v>1</v>
+      </c>
+      <c r="G10" s="24">
+        <v>0</v>
+      </c>
+      <c r="H10" s="24">
+        <v>0</v>
+      </c>
+      <c r="I10" s="24">
+        <v>1</v>
+      </c>
+      <c r="J10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="15">
+      <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="D11" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="18">
-        <v>1</v>
-      </c>
-      <c r="F11" s="30">
-        <v>0</v>
-      </c>
-      <c r="G11" s="18">
-        <v>0</v>
-      </c>
-      <c r="H11" s="18">
-        <v>1</v>
-      </c>
-      <c r="I11" s="23"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A12" s="19" t="s">
+      <c r="F11" s="24">
+        <v>1</v>
+      </c>
+      <c r="G11" s="24">
+        <v>0</v>
+      </c>
+      <c r="H11" s="24">
+        <v>0</v>
+      </c>
+      <c r="I11" s="24">
+        <v>1</v>
+      </c>
+      <c r="J11" s="20"/>
+    </row>
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="15">
+      <c r="A12" s="6" t="s">
         <v>99</v>
       </c>
       <c r="B12" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="D12" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="E12" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="18">
-        <v>1</v>
-      </c>
-      <c r="F12" s="30">
-        <v>0</v>
-      </c>
-      <c r="G12" s="18">
-        <v>0</v>
-      </c>
-      <c r="H12" s="18">
-        <v>1</v>
-      </c>
-      <c r="I12" s="14"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A13" s="19" t="s">
+      <c r="F12" s="24">
+        <v>1</v>
+      </c>
+      <c r="G12" s="24">
+        <v>0</v>
+      </c>
+      <c r="H12" s="24">
+        <v>0</v>
+      </c>
+      <c r="I12" s="24">
+        <v>1</v>
+      </c>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="15">
+      <c r="A13" s="6" t="s">
         <v>100</v>
       </c>
       <c r="B13" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="D13" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="E13" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="18">
-        <v>1</v>
-      </c>
-      <c r="F13" s="30">
-        <v>0</v>
-      </c>
-      <c r="G13" s="18">
-        <v>0</v>
-      </c>
-      <c r="H13" s="18">
-        <v>1</v>
-      </c>
-      <c r="I13" s="14"/>
-    </row>
-    <row r="14" spans="1:10" s="15" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A14" s="19" t="s">
+      <c r="F13" s="24">
+        <v>1</v>
+      </c>
+      <c r="G13" s="24">
+        <v>0</v>
+      </c>
+      <c r="H13" s="24">
+        <v>0</v>
+      </c>
+      <c r="I13" s="24">
+        <v>1</v>
+      </c>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:11" s="35" customFormat="1" ht="15">
+      <c r="A14" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="D14" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="E14" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="E14" s="31">
-        <v>1</v>
-      </c>
-      <c r="F14" s="30">
-        <v>0</v>
-      </c>
-      <c r="G14" s="18">
-        <v>0</v>
-      </c>
-      <c r="H14" s="18">
-        <v>1</v>
-      </c>
-      <c r="I14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A15" s="19" t="s">
+      <c r="F14" s="34">
+        <v>1</v>
+      </c>
+      <c r="G14" s="24">
+        <v>0</v>
+      </c>
+      <c r="H14" s="24">
+        <v>0</v>
+      </c>
+      <c r="I14" s="24">
+        <v>1</v>
+      </c>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="1:11" s="33" customFormat="1" ht="15">
+      <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="D15" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="18">
-        <v>1</v>
-      </c>
-      <c r="F15" s="30">
-        <v>0</v>
-      </c>
-      <c r="G15" s="18">
-        <v>0</v>
-      </c>
-      <c r="H15" s="18">
-        <v>1</v>
-      </c>
-      <c r="I15" s="14"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A16" s="19" t="s">
+      <c r="F15" s="24">
+        <v>1</v>
+      </c>
+      <c r="G15" s="24">
+        <v>0</v>
+      </c>
+      <c r="H15" s="24">
+        <v>0</v>
+      </c>
+      <c r="I15" s="24">
+        <v>1</v>
+      </c>
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:11" s="33" customFormat="1" ht="15">
+      <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="D16" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="E16" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="18">
-        <v>1</v>
-      </c>
-      <c r="F16" s="30">
-        <v>0</v>
-      </c>
-      <c r="G16" s="18">
-        <v>0</v>
-      </c>
-      <c r="H16" s="18">
-        <v>1</v>
-      </c>
-      <c r="I16" s="14"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A17" s="19" t="s">
+      <c r="F16" s="24">
+        <v>1</v>
+      </c>
+      <c r="G16" s="24">
+        <v>0</v>
+      </c>
+      <c r="H16" s="24">
+        <v>0</v>
+      </c>
+      <c r="I16" s="24">
+        <v>1</v>
+      </c>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="D17" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="E17" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="18">
-        <v>1</v>
-      </c>
-      <c r="F17" s="30">
-        <v>0</v>
-      </c>
-      <c r="G17" s="18">
-        <v>0</v>
-      </c>
-      <c r="H17" s="18">
-        <v>1</v>
-      </c>
-      <c r="I17" s="14"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A18" s="19" t="s">
+      <c r="F17" s="24">
+        <v>1</v>
+      </c>
+      <c r="G17" s="24">
+        <v>0</v>
+      </c>
+      <c r="H17" s="24">
+        <v>0</v>
+      </c>
+      <c r="I17" s="24">
+        <v>1</v>
+      </c>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="D18" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="E18" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="18">
-        <v>1</v>
-      </c>
-      <c r="F18" s="30">
-        <v>0</v>
-      </c>
-      <c r="G18" s="18">
-        <v>0</v>
-      </c>
-      <c r="H18" s="18">
-        <v>1</v>
-      </c>
-      <c r="I18" s="14"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A19" s="19" t="s">
+      <c r="F18" s="24">
+        <v>1</v>
+      </c>
+      <c r="G18" s="24">
+        <v>0</v>
+      </c>
+      <c r="H18" s="24">
+        <v>0</v>
+      </c>
+      <c r="I18" s="24">
+        <v>1</v>
+      </c>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10" s="33" customFormat="1" ht="30">
+      <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="D19" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="E19" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="18">
-        <v>1</v>
-      </c>
-      <c r="F19" s="30">
-        <v>0</v>
-      </c>
-      <c r="G19" s="18">
-        <v>0</v>
-      </c>
-      <c r="H19" s="18">
-        <v>0</v>
-      </c>
-      <c r="I19" s="24"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A20" s="19" t="s">
+      <c r="F19" s="24">
+        <v>1</v>
+      </c>
+      <c r="G19" s="24">
+        <v>0</v>
+      </c>
+      <c r="H19" s="24">
+        <v>0</v>
+      </c>
+      <c r="I19" s="24">
+        <v>0</v>
+      </c>
+      <c r="J19" s="21"/>
+    </row>
+    <row r="20" spans="1:10" s="33" customFormat="1" ht="30">
+      <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="D20" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="E20" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="18">
-        <v>1</v>
-      </c>
-      <c r="F20" s="30">
-        <v>0</v>
-      </c>
-      <c r="G20" s="18">
-        <v>0</v>
-      </c>
-      <c r="H20" s="18">
-        <v>0</v>
-      </c>
-      <c r="I20" s="24"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A21" s="19" t="s">
+      <c r="F20" s="24">
+        <v>1</v>
+      </c>
+      <c r="G20" s="24">
+        <v>0</v>
+      </c>
+      <c r="H20" s="24">
+        <v>0</v>
+      </c>
+      <c r="I20" s="24">
+        <v>0</v>
+      </c>
+      <c r="J20" s="21"/>
+    </row>
+    <row r="21" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="D21" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="E21" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="18">
-        <v>1</v>
-      </c>
-      <c r="F21" s="30">
-        <v>0</v>
-      </c>
-      <c r="G21" s="18">
-        <v>0</v>
-      </c>
-      <c r="H21" s="18">
-        <v>0</v>
-      </c>
-      <c r="I21" s="24"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A22" s="19" t="s">
+      <c r="F21" s="24">
+        <v>1</v>
+      </c>
+      <c r="G21" s="24">
+        <v>0</v>
+      </c>
+      <c r="H21" s="24">
+        <v>0</v>
+      </c>
+      <c r="I21" s="24">
+        <v>0</v>
+      </c>
+      <c r="J21" s="21"/>
+    </row>
+    <row r="22" spans="1:10" s="33" customFormat="1" ht="30">
+      <c r="A22" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="D22" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="E22" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="18">
-        <v>1</v>
-      </c>
-      <c r="F22" s="30">
-        <v>0</v>
-      </c>
-      <c r="G22" s="18">
-        <v>0</v>
-      </c>
-      <c r="H22" s="18">
-        <v>0</v>
-      </c>
-      <c r="I22" s="24"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A23" s="19" t="s">
+      <c r="F22" s="24">
+        <v>1</v>
+      </c>
+      <c r="G22" s="24">
+        <v>0</v>
+      </c>
+      <c r="H22" s="24">
+        <v>0</v>
+      </c>
+      <c r="I22" s="24">
+        <v>0</v>
+      </c>
+      <c r="J22" s="21"/>
+    </row>
+    <row r="23" spans="1:10" s="33" customFormat="1" ht="30">
+      <c r="A23" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="D23" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="E23" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="18">
-        <v>1</v>
-      </c>
-      <c r="F23" s="30">
-        <v>0</v>
-      </c>
-      <c r="G23" s="18">
-        <v>0</v>
-      </c>
-      <c r="H23" s="18">
-        <v>0</v>
-      </c>
-      <c r="I23" s="24"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A24" s="19" t="s">
+      <c r="F23" s="24">
+        <v>1</v>
+      </c>
+      <c r="G23" s="24">
+        <v>0</v>
+      </c>
+      <c r="H23" s="24">
+        <v>0</v>
+      </c>
+      <c r="I23" s="24">
+        <v>0</v>
+      </c>
+      <c r="J23" s="21"/>
+    </row>
+    <row r="24" spans="1:10" s="33" customFormat="1" ht="30">
+      <c r="A24" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="D24" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="E24" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="18">
-        <v>1</v>
-      </c>
-      <c r="F24" s="30">
-        <v>0</v>
-      </c>
-      <c r="G24" s="18">
-        <v>0</v>
-      </c>
-      <c r="H24" s="18">
-        <v>0</v>
-      </c>
-      <c r="I24" s="24"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A25" s="19" t="s">
+      <c r="F24" s="24">
+        <v>1</v>
+      </c>
+      <c r="G24" s="24">
+        <v>0</v>
+      </c>
+      <c r="H24" s="24">
+        <v>0</v>
+      </c>
+      <c r="I24" s="24">
+        <v>0</v>
+      </c>
+      <c r="J24" s="21"/>
+    </row>
+    <row r="25" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="D25" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="E25" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="18">
-        <v>1</v>
-      </c>
-      <c r="F25" s="30">
-        <v>0</v>
-      </c>
-      <c r="G25" s="18">
-        <v>0</v>
-      </c>
-      <c r="H25" s="18">
-        <v>0</v>
-      </c>
-      <c r="I25" s="24"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A26" s="19" t="s">
+      <c r="F25" s="24">
+        <v>1</v>
+      </c>
+      <c r="G25" s="24">
+        <v>0</v>
+      </c>
+      <c r="H25" s="24">
+        <v>0</v>
+      </c>
+      <c r="I25" s="24">
+        <v>0</v>
+      </c>
+      <c r="J25" s="21"/>
+    </row>
+    <row r="26" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A26" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="D26" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="E26" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="18">
-        <v>1</v>
-      </c>
-      <c r="F26" s="30">
-        <v>0</v>
-      </c>
-      <c r="G26" s="18">
-        <v>0</v>
-      </c>
-      <c r="H26" s="18">
-        <v>0</v>
-      </c>
-      <c r="I26" s="24"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A27" s="19" t="s">
+      <c r="F26" s="24">
+        <v>1</v>
+      </c>
+      <c r="G26" s="24">
+        <v>0</v>
+      </c>
+      <c r="H26" s="24">
+        <v>0</v>
+      </c>
+      <c r="I26" s="24">
+        <v>0</v>
+      </c>
+      <c r="J26" s="21"/>
+    </row>
+    <row r="27" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="D27" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="E27" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="18">
-        <v>1</v>
-      </c>
-      <c r="F27" s="30">
-        <v>0</v>
-      </c>
-      <c r="G27" s="18">
-        <v>0</v>
-      </c>
-      <c r="H27" s="18">
-        <v>0</v>
-      </c>
-      <c r="I27" s="24"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A28" s="19" t="s">
+      <c r="F27" s="24">
+        <v>1</v>
+      </c>
+      <c r="G27" s="24">
+        <v>0</v>
+      </c>
+      <c r="H27" s="24">
+        <v>0</v>
+      </c>
+      <c r="I27" s="24">
+        <v>0</v>
+      </c>
+      <c r="J27" s="21"/>
+    </row>
+    <row r="28" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A28" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="C28" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="D28" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="18">
-        <v>1</v>
-      </c>
-      <c r="F28" s="30">
-        <v>0</v>
-      </c>
-      <c r="G28" s="18">
-        <v>0</v>
-      </c>
-      <c r="H28" s="18">
-        <v>0</v>
-      </c>
-      <c r="I28" s="14"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A29" s="19" t="s">
+      <c r="E28" s="14"/>
+      <c r="F28" s="24">
+        <v>1</v>
+      </c>
+      <c r="G28" s="24">
+        <v>0</v>
+      </c>
+      <c r="H28" s="24">
+        <v>0</v>
+      </c>
+      <c r="I28" s="24">
+        <v>0</v>
+      </c>
+      <c r="J28" s="14"/>
+    </row>
+    <row r="29" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A29" s="6" t="s">
         <v>84</v>
       </c>
       <c r="B29" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="D29" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="E29" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="18">
-        <v>1</v>
-      </c>
-      <c r="F29" s="30">
-        <v>0</v>
-      </c>
-      <c r="G29" s="18">
-        <v>0</v>
-      </c>
-      <c r="H29" s="18">
-        <v>0</v>
-      </c>
-      <c r="I29" s="14"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A30" s="19" t="s">
+      <c r="F29" s="24">
+        <v>1</v>
+      </c>
+      <c r="G29" s="24">
+        <v>0</v>
+      </c>
+      <c r="H29" s="24">
+        <v>0</v>
+      </c>
+      <c r="I29" s="24">
+        <v>0</v>
+      </c>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A30" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="D30" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="18">
-        <v>1</v>
-      </c>
-      <c r="F30" s="30">
-        <v>0</v>
-      </c>
-      <c r="G30" s="18">
-        <v>0</v>
-      </c>
-      <c r="H30" s="18">
-        <v>1</v>
-      </c>
-      <c r="I30" s="14"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A31" s="19" t="s">
+      <c r="E30" s="14"/>
+      <c r="F30" s="24">
+        <v>1</v>
+      </c>
+      <c r="G30" s="24">
+        <v>0</v>
+      </c>
+      <c r="H30" s="24">
+        <v>0</v>
+      </c>
+      <c r="I30" s="24">
+        <v>1</v>
+      </c>
+      <c r="J30" s="14"/>
+    </row>
+    <row r="31" spans="1:10" s="33" customFormat="1" ht="30">
+      <c r="A31" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C31" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="D31" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="18">
-        <v>1</v>
-      </c>
-      <c r="F31" s="30">
-        <v>0</v>
-      </c>
-      <c r="G31" s="18">
-        <v>0</v>
-      </c>
-      <c r="H31" s="18">
-        <v>1</v>
-      </c>
-      <c r="I31" s="14"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A32" s="19" t="s">
+      <c r="E31" s="14"/>
+      <c r="F31" s="24">
+        <v>1</v>
+      </c>
+      <c r="G31" s="24">
+        <v>0</v>
+      </c>
+      <c r="H31" s="24">
+        <v>0</v>
+      </c>
+      <c r="I31" s="24">
+        <v>1</v>
+      </c>
+      <c r="J31" s="14"/>
+    </row>
+    <row r="32" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A32" s="6" t="s">
         <v>81</v>
       </c>
       <c r="B32" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="D32" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="E32" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="18">
-        <v>1</v>
-      </c>
-      <c r="F32" s="30">
-        <v>0</v>
-      </c>
-      <c r="G32" s="18">
-        <v>0</v>
-      </c>
-      <c r="H32" s="18">
-        <v>0</v>
-      </c>
-      <c r="I32" s="14"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A33" s="19" t="s">
+      <c r="F32" s="24">
+        <v>1</v>
+      </c>
+      <c r="G32" s="24">
+        <v>0</v>
+      </c>
+      <c r="H32" s="24">
+        <v>0</v>
+      </c>
+      <c r="I32" s="24">
+        <v>0</v>
+      </c>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A33" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="D33" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="18">
-        <v>1</v>
-      </c>
-      <c r="F33" s="30">
-        <v>0</v>
-      </c>
-      <c r="G33" s="18">
-        <v>0</v>
-      </c>
-      <c r="H33" s="18">
-        <v>0</v>
-      </c>
-      <c r="I33" s="14" t="s">
+      <c r="E33" s="14"/>
+      <c r="F33" s="24">
+        <v>1</v>
+      </c>
+      <c r="G33" s="24">
+        <v>0</v>
+      </c>
+      <c r="H33" s="24">
+        <v>0</v>
+      </c>
+      <c r="I33" s="24">
+        <v>0</v>
+      </c>
+      <c r="J33" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A34" s="19" t="s">
+    <row r="34" spans="1:10" s="33" customFormat="1" ht="30">
+      <c r="A34" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="D34" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="D34" s="14"/>
-      <c r="E34" s="18">
-        <v>1</v>
-      </c>
-      <c r="F34" s="30">
-        <v>0</v>
-      </c>
-      <c r="G34" s="18">
-        <v>0</v>
-      </c>
-      <c r="H34" s="18">
-        <v>0</v>
-      </c>
-      <c r="I34" s="14" t="s">
+      <c r="E34" s="14"/>
+      <c r="F34" s="24">
+        <v>1</v>
+      </c>
+      <c r="G34" s="24">
+        <v>0</v>
+      </c>
+      <c r="H34" s="24">
+        <v>0</v>
+      </c>
+      <c r="I34" s="24">
+        <v>0</v>
+      </c>
+      <c r="J34" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A35" s="19" t="s">
+    <row r="35" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A35" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="D35" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="18">
-        <v>0</v>
-      </c>
-      <c r="F35" s="30">
-        <v>0</v>
-      </c>
-      <c r="G35" s="18">
-        <v>0</v>
-      </c>
-      <c r="H35" s="18">
-        <v>0</v>
-      </c>
-      <c r="I35" s="14"/>
-    </row>
-    <row r="36" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A36" s="19" t="s">
+      <c r="E35" s="14"/>
+      <c r="F35" s="24">
+        <v>0</v>
+      </c>
+      <c r="G35" s="24">
+        <v>0</v>
+      </c>
+      <c r="H35" s="24">
+        <v>0</v>
+      </c>
+      <c r="I35" s="24">
+        <v>0</v>
+      </c>
+      <c r="J35" s="14"/>
+    </row>
+    <row r="36" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A36" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="D36" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="14"/>
-      <c r="E36" s="18">
-        <v>0</v>
-      </c>
-      <c r="F36" s="30">
-        <v>0</v>
-      </c>
-      <c r="G36" s="18">
-        <v>0</v>
-      </c>
-      <c r="H36" s="18">
-        <v>0</v>
-      </c>
-      <c r="I36" s="14"/>
-    </row>
-    <row r="37" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A37" s="19" t="s">
+      <c r="E36" s="14"/>
+      <c r="F36" s="24">
+        <v>0</v>
+      </c>
+      <c r="G36" s="24">
+        <v>0</v>
+      </c>
+      <c r="H36" s="24">
+        <v>0</v>
+      </c>
+      <c r="I36" s="24">
+        <v>0</v>
+      </c>
+      <c r="J36" s="14"/>
+    </row>
+    <row r="37" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A37" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="C37" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="D37" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D37" s="14"/>
-      <c r="E37" s="18">
-        <v>0</v>
-      </c>
-      <c r="F37" s="30">
-        <v>0</v>
-      </c>
-      <c r="G37" s="18">
-        <v>0</v>
-      </c>
-      <c r="H37" s="18">
-        <v>0</v>
-      </c>
-      <c r="I37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="24">
+        <v>0</v>
+      </c>
+      <c r="G37" s="24">
+        <v>0</v>
+      </c>
+      <c r="H37" s="24">
+        <v>0</v>
+      </c>
+      <c r="I37" s="24">
+        <v>0</v>
+      </c>
+      <c r="J37" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E1:H1048576">
+  <conditionalFormatting sqref="F1:I1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:H499">
+  <conditionalFormatting sqref="F3:I499">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="whole" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="E5:H37">
+    <dataValidation type="whole" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="F5:I37">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
ASKAPSDP-2214 working on VOTable data parsing code generation
</commit_message>
<xml_diff>
--- a/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
+++ b/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
@@ -32,8 +32,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:
-</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="178">
   <si>
     <t>gsm.continuum_component 
 10 November 2016</t>
@@ -160,7 +159,7 @@
     <t>pos.eq.dec</t>
   </si>
   <si>
-    <t>J2000 declination (dd:mm:ss.ss) </t>
+    <t>J2000 declination (dd:mm:ss.ss)</t>
   </si>
   <si>
     <t>deg:arcmin:arcsec</t>
@@ -220,7 +219,7 @@
     <t>em.freq</t>
   </si>
   <si>
-    <t>Frequency </t>
+    <t>Frequency</t>
   </si>
   <si>
     <t>MHz</t>
@@ -232,7 +231,7 @@
     <t>phot.flux.density;stat.max;em.radio;stat.fit</t>
   </si>
   <si>
-    <t>Peak flux density </t>
+    <t>Peak flux density</t>
   </si>
   <si>
     <t>mJy/beam</t>
@@ -404,9 +403,6 @@
   </si>
   <si>
     <t>BOOLEAN</t>
-  </si>
-  <si>
-    <t>Can this be a BOOLEAN?</t>
   </si>
   <si>
     <t>fit_is_estimate</t>
@@ -745,7 +741,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -835,18 +831,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -856,10 +840,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -886,7 +866,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -954,7 +934,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFC6EFCE"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFEB9C"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -988,8 +968,8 @@
   </sheetPr>
   <dimension ref="1:37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
@@ -11518,23 +11498,23 @@
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="23" t="n">
+      <c r="F14" s="15" t="n">
         <v>1</v>
       </c>
       <c r="G14" s="15" t="n">
@@ -11546,7 +11526,7 @@
       <c r="I14" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="J14" s="22"/>
+      <c r="J14" s="14"/>
     </row>
     <row r="15" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
@@ -11696,7 +11676,7 @@
       <c r="I19" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J19" s="25"/>
+      <c r="J19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
@@ -11726,7 +11706,7 @@
       <c r="I20" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J20" s="25"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
@@ -11756,7 +11736,7 @@
       <c r="I21" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J21" s="25"/>
+      <c r="J21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
@@ -11786,7 +11766,7 @@
       <c r="I22" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J22" s="25"/>
+      <c r="J22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
@@ -11816,7 +11796,7 @@
       <c r="I23" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J23" s="25"/>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
@@ -11846,7 +11826,7 @@
       <c r="I24" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J24" s="25"/>
+      <c r="J24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
@@ -11876,7 +11856,7 @@
       <c r="I25" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J25" s="25"/>
+      <c r="J25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
@@ -11906,7 +11886,7 @@
       <c r="I26" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J26" s="25"/>
+      <c r="J26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
@@ -11936,7 +11916,7 @@
       <c r="I27" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J27" s="25"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="16" t="s">
@@ -12108,19 +12088,17 @@
       <c r="I33" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J33" s="14" t="s">
+      <c r="J33" s="14"/>
+    </row>
+    <row r="34" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="16" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="16" t="s">
-        <v>118</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>114</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>116</v>
@@ -12138,22 +12116,20 @@
       <c r="I34" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J34" s="14" t="s">
-        <v>117</v>
-      </c>
+      <c r="J34" s="14"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B35" s="14" t="s">
         <v>114</v>
       </c>
       <c r="C35" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>122</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="15" t="n">
@@ -12172,16 +12148,16 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>114</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="15" t="n">
@@ -12200,16 +12176,16 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="C37" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="D37" s="14" t="s">
         <v>127</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>128</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="15" t="n">
@@ -12230,13 +12206,8 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F:I">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F3:I499">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12264,7 +12235,7 @@
   </sheetPr>
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -12282,604 +12253,604 @@
       <c r="E1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="C2" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="D2" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="E2" s="23" t="s">
         <v>132</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="17"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="16"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="C4" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>136</v>
+      <c r="D4" s="25" t="s">
+        <v>135</v>
       </c>
       <c r="E4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>136</v>
+      <c r="C5" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>135</v>
       </c>
       <c r="E5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29" t="s">
-        <v>139</v>
+      <c r="A6" s="25" t="s">
+        <v>138</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>136</v>
+      <c r="C6" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>135</v>
       </c>
       <c r="E6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>136</v>
+      <c r="C7" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>135</v>
       </c>
       <c r="E7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>136</v>
+      <c r="C8" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>135</v>
       </c>
       <c r="E8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="17"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
       <c r="E9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29" t="n">
+      <c r="A10" s="25" t="n">
         <v>1</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>136</v>
+      <c r="C10" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>135</v>
       </c>
       <c r="E10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29" t="n">
+      <c r="A11" s="25" t="n">
         <v>2</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>136</v>
+      <c r="C11" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>135</v>
       </c>
       <c r="E11" s="16"/>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="29" t="n">
+      <c r="A12" s="25" t="n">
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D12" s="29"/>
+      <c r="C12" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="25"/>
       <c r="E12" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29" t="n">
+      <c r="A13" s="25" t="n">
         <v>4</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D13" s="29"/>
+        <v>146</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" s="25"/>
       <c r="E13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="29" t="n">
+      <c r="A14" s="25" t="n">
         <v>5</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="D14" s="29" t="s">
+      <c r="C14" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>41</v>
       </c>
       <c r="E14" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="29" t="n">
+      <c r="A15" s="25" t="n">
         <v>6</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="D15" s="29" t="s">
+      <c r="C15" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="25" t="s">
         <v>41</v>
       </c>
       <c r="E15" s="16"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="29" t="n">
+      <c r="A16" s="25" t="n">
         <v>7</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D16" s="29"/>
+        <v>149</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" s="25"/>
       <c r="E16" s="16"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="29" t="n">
+      <c r="A17" s="25" t="n">
         <v>8</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D17" s="29"/>
+        <v>150</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="25"/>
       <c r="E17" s="16"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="29" t="n">
+      <c r="A18" s="25" t="n">
         <v>9</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>152</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>153</v>
       </c>
       <c r="E18" s="16"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="29" t="n">
+      <c r="A19" s="25" t="n">
         <v>10</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D19" s="29"/>
+      <c r="C19" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="25"/>
       <c r="E19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="29" t="n">
+      <c r="A20" s="25" t="n">
         <v>11</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="25" t="s">
         <v>154</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>155</v>
       </c>
       <c r="E20" s="16"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="29" t="n">
+      <c r="A21" s="25" t="n">
         <v>12</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21" s="29"/>
+      <c r="C21" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="25"/>
       <c r="E21" s="16"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="29" t="n">
+      <c r="A22" s="25" t="n">
         <v>13</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="D22" s="29" t="s">
+      <c r="C22" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="D22" s="25" t="s">
         <v>49</v>
       </c>
       <c r="E22" s="16"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="29" t="n">
+      <c r="A23" s="25" t="n">
         <v>14</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="D23" s="29" t="s">
+      <c r="C23" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="16"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="29" t="n">
+      <c r="A24" s="25" t="n">
         <v>15</v>
       </c>
       <c r="B24" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="D24" s="29" t="s">
+      <c r="C24" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="D24" s="25" t="s">
         <v>41</v>
       </c>
       <c r="E24" s="16"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="29" t="n">
+      <c r="A25" s="25" t="n">
         <v>16</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="D25" s="29" t="s">
+      <c r="C25" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="25" t="s">
         <v>49</v>
       </c>
       <c r="E25" s="16"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="29" t="n">
+      <c r="A26" s="25" t="n">
         <v>17</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C26" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="D26" s="29" t="s">
+      <c r="C26" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" s="25" t="s">
         <v>49</v>
       </c>
       <c r="E26" s="16"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="29" t="n">
+      <c r="A27" s="25" t="n">
         <v>18</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="D27" s="29" t="s">
+      <c r="C27" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D27" s="25" t="s">
         <v>41</v>
       </c>
       <c r="E27" s="16"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="29" t="n">
+      <c r="A28" s="25" t="n">
         <v>19</v>
       </c>
       <c r="B28" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>136</v>
+      <c r="C28" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>135</v>
       </c>
       <c r="E28" s="16"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="29" t="n">
+      <c r="A29" s="25" t="n">
         <v>20</v>
       </c>
       <c r="B29" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="D29" s="29" t="s">
+      <c r="C29" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" s="25" t="s">
         <v>60</v>
       </c>
       <c r="E29" s="16"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="29" t="n">
+      <c r="A30" s="25" t="n">
         <v>21</v>
       </c>
       <c r="B30" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D30" s="29"/>
+      <c r="C30" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="25"/>
       <c r="E30" s="16"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="29" t="n">
+      <c r="A31" s="25" t="n">
         <v>22</v>
       </c>
       <c r="B31" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="C31" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D31" s="29"/>
+      <c r="C31" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" s="25"/>
       <c r="E31" s="16"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="29" t="n">
+      <c r="A32" s="25" t="n">
         <v>23</v>
       </c>
       <c r="B32" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C32" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>153</v>
+      <c r="C32" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>152</v>
       </c>
       <c r="E32" s="16"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="29" t="n">
+      <c r="A33" s="25" t="n">
         <v>24</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="C33" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D33" s="29"/>
+        <v>164</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33" s="25"/>
       <c r="E33" s="16"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="29" t="n">
+      <c r="A34" s="25" t="n">
         <v>25</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D34" s="29"/>
+        <v>165</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" s="25"/>
       <c r="E34" s="16"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="29" t="n">
+      <c r="A35" s="25" t="n">
         <v>26</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D35" s="29"/>
+        <v>119</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D35" s="25"/>
       <c r="E35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="29" t="n">
+      <c r="A36" s="25" t="n">
         <v>27</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C36" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D36" s="29"/>
+        <v>122</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" s="25"/>
       <c r="E36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="29" t="n">
+      <c r="A37" s="25" t="n">
         <v>28</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D37" s="29"/>
+        <v>124</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37" s="25"/>
       <c r="E37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="30" t="n">
+      <c r="A38" s="26" t="n">
         <v>29</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="D38" s="29"/>
+      <c r="C38" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" s="25"/>
       <c r="E38" s="16"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="30" t="n">
+      <c r="A39" s="26" t="n">
         <v>30</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="D39" s="29"/>
+      <c r="C39" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" s="25"/>
       <c r="E39" s="16"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="30" t="n">
+      <c r="A40" s="26" t="n">
         <v>31</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="D40" s="29"/>
+      <c r="C40" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D40" s="25"/>
       <c r="E40" s="16"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="32" t="s">
-        <v>167</v>
+      <c r="D41" s="28" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D42" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D43" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D44" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D45" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D46" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D47" s="0" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D48" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D49" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D50" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D51" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D52" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ASKAPSDP-2214 first version of component VOTable parsing with generated code done. Most tests passing
</commit_message>
<xml_diff>
--- a/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
+++ b/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
@@ -866,23 +866,9 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <sz val="11"/>
@@ -909,7 +895,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF9C0006"/>
-      <rgbColor rgb="FF006100"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF9C6500"/>
       <rgbColor rgb="FF800080"/>
@@ -969,7 +955,7 @@
   <dimension ref="1:37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
@@ -11528,7 +11514,7 @@
       </c>
       <c r="J14" s="14"/>
     </row>
-    <row r="15" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
         <v>57</v>
       </c>
@@ -11558,7 +11544,7 @@
       </c>
       <c r="J15" s="14"/>
     </row>
-    <row r="16" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
         <v>61</v>
       </c>
@@ -11588,7 +11574,7 @@
       </c>
       <c r="J16" s="14"/>
     </row>
-    <row r="17" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="s">
         <v>64</v>
       </c>
@@ -11618,7 +11604,7 @@
       </c>
       <c r="J17" s="14"/>
     </row>
-    <row r="18" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
         <v>68</v>
       </c>
@@ -12207,7 +12193,7 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:I499">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ASKAPSDP-2214 implemented polarisation data ingest
</commit_message>
<xml_diff>
--- a/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
+++ b/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
@@ -866,7 +866,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -955,7 +955,7 @@
   <dimension ref="1:37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
@@ -3047,7 +3047,7 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="2" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
ASKAPSDP-2214 unit test for ingest of non-ASKAP sources
</commit_message>
<xml_diff>
--- a/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
+++ b/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="179">
   <si>
     <t>gsm.continuum_component 
 10 November 2016</t>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Posix Date-time</t>
+  </si>
+  <si>
+    <t>For ASKAP sources, this is the date of the observation. For non-ASKAP sources, this field is NULL.</t>
   </si>
   <si>
     <t>healpix_index</t>
@@ -866,7 +869,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -955,7 +958,7 @@
   <dimension ref="1:37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
@@ -3047,7 +3050,7 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="2" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="2" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
@@ -3073,18 +3076,20 @@
       <c r="I3" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J3" s="14"/>
+      <c r="J3" s="14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="15" t="n">
@@ -3100,19 +3105,19 @@
         <v>1</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="15" t="n">
@@ -3132,16 +3137,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="15" t="n">
@@ -4174,16 +4179,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>24</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="15" t="n">
@@ -4199,7 +4204,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K7" s="0"/>
       <c r="L7" s="0"/>
@@ -5218,19 +5223,19 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" s="15" t="n">
         <v>0</v>
@@ -5245,7 +5250,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K8" s="0"/>
       <c r="L8" s="0"/>
@@ -6264,19 +6269,19 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F9" s="15" t="n">
         <v>0</v>
@@ -6291,7 +6296,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K9" s="0"/>
       <c r="L9" s="0"/>
@@ -7310,19 +7315,19 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F10" s="15" t="n">
         <v>1</v>
@@ -8354,19 +8359,19 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>42</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>41</v>
       </c>
       <c r="F11" s="15" t="n">
         <v>1</v>
@@ -9398,19 +9403,19 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F12" s="15" t="n">
         <v>1</v>
@@ -10442,19 +10447,19 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>49</v>
       </c>
       <c r="F13" s="15" t="n">
         <v>1</v>
@@ -11486,19 +11491,19 @@
     </row>
     <row r="14" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F14" s="15" t="n">
         <v>1</v>
@@ -11516,19 +11521,19 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F15" s="15" t="n">
         <v>1</v>
@@ -11546,19 +11551,19 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>60</v>
       </c>
       <c r="F16" s="15" t="n">
         <v>1</v>
@@ -11576,19 +11581,19 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F17" s="15" t="n">
         <v>1</v>
@@ -11606,19 +11611,19 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>68</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>67</v>
       </c>
       <c r="F18" s="15" t="n">
         <v>1</v>
@@ -11636,19 +11641,19 @@
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F19" s="15" t="n">
         <v>1</v>
@@ -11666,19 +11671,19 @@
     </row>
     <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F20" s="15" t="n">
         <v>1</v>
@@ -11696,19 +11701,19 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F21" s="15" t="n">
         <v>1</v>
@@ -11726,19 +11731,19 @@
     </row>
     <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F22" s="15" t="n">
         <v>1</v>
@@ -11756,19 +11761,19 @@
     </row>
     <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F23" s="15" t="n">
         <v>1</v>
@@ -11786,19 +11791,19 @@
     </row>
     <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F24" s="15" t="n">
         <v>1</v>
@@ -11816,19 +11821,19 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F25" s="15" t="n">
         <v>1</v>
@@ -11846,19 +11851,19 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F26" s="15" t="n">
         <v>1</v>
@@ -11876,19 +11881,19 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F27" s="15" t="n">
         <v>1</v>
@@ -11906,16 +11911,16 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="15" t="n">
@@ -11934,19 +11939,19 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F29" s="15" t="n">
         <v>1</v>
@@ -11964,16 +11969,16 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="15" t="n">
@@ -11992,16 +11997,16 @@
     </row>
     <row r="31" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="15" t="n">
@@ -12020,19 +12025,19 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F32" s="15" t="n">
         <v>1</v>
@@ -12050,16 +12055,16 @@
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="15" t="n">
@@ -12078,16 +12083,16 @@
     </row>
     <row r="34" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" s="14" t="s">
         <v>117</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>116</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="15" t="n">
@@ -12106,16 +12111,16 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="15" t="n">
@@ -12134,16 +12139,16 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D36" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>121</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="15" t="n">
@@ -12162,16 +12167,16 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="15" t="n">
@@ -12240,19 +12245,19 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12264,76 +12269,76 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>135</v>
-      </c>
       <c r="D5" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="25" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="25" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E8" s="16"/>
     </row>
@@ -12349,13 +12354,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E10" s="16"/>
     </row>
@@ -12364,13 +12369,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E11" s="16"/>
     </row>
@@ -12379,14 +12384,14 @@
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12394,10 +12399,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="16"/>
@@ -12407,13 +12412,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E14" s="16"/>
     </row>
@@ -12422,13 +12427,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="25" t="s">
         <v>42</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>41</v>
       </c>
       <c r="E15" s="16"/>
     </row>
@@ -12437,10 +12442,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="16"/>
@@ -12450,10 +12455,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="16"/>
@@ -12463,13 +12468,13 @@
         <v>9</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E18" s="16"/>
     </row>
@@ -12478,10 +12483,10 @@
         <v>10</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="16"/>
@@ -12491,13 +12496,13 @@
         <v>11</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E20" s="16"/>
     </row>
@@ -12506,10 +12511,10 @@
         <v>12</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="16"/>
@@ -12519,13 +12524,13 @@
         <v>13</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E22" s="16"/>
     </row>
@@ -12534,13 +12539,13 @@
         <v>14</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E23" s="16"/>
     </row>
@@ -12549,13 +12554,13 @@
         <v>15</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E24" s="16"/>
     </row>
@@ -12564,13 +12569,13 @@
         <v>16</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E25" s="16"/>
     </row>
@@ -12579,13 +12584,13 @@
         <v>17</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E26" s="16"/>
     </row>
@@ -12594,13 +12599,13 @@
         <v>18</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E27" s="16"/>
     </row>
@@ -12609,13 +12614,13 @@
         <v>19</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E28" s="16"/>
     </row>
@@ -12624,13 +12629,13 @@
         <v>20</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E29" s="16"/>
     </row>
@@ -12639,10 +12644,10 @@
         <v>21</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="16"/>
@@ -12652,10 +12657,10 @@
         <v>22</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="16"/>
@@ -12665,13 +12670,13 @@
         <v>23</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E32" s="16"/>
     </row>
@@ -12680,10 +12685,10 @@
         <v>24</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D33" s="25"/>
       <c r="E33" s="16"/>
@@ -12693,10 +12698,10 @@
         <v>25</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="16"/>
@@ -12706,10 +12711,10 @@
         <v>26</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="16"/>
@@ -12719,10 +12724,10 @@
         <v>27</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="16"/>
@@ -12732,10 +12737,10 @@
         <v>28</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="16"/>
@@ -12745,10 +12750,10 @@
         <v>29</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="16"/>
@@ -12758,10 +12763,10 @@
         <v>30</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D39" s="25"/>
       <c r="E39" s="16"/>
@@ -12771,72 +12776,72 @@
         <v>31</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="16"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D41" s="28" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D42" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D43" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D44" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D45" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D46" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D47" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D48" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D49" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D50" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D51" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D52" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ASKAPSDP-2215 unit test for simple cone search, and stub functions
</commit_message>
<xml_diff>
--- a/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
+++ b/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="181">
   <si>
     <t>gsm.continuum_component 
 10 November 2016</t>
@@ -168,337 +168,343 @@
     <t>deg:arcmin:arcsec</t>
   </si>
   <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>pos.eq.ra;meta.main</t>
+  </si>
+  <si>
+    <t>J2000 right ascension</t>
+  </si>
+  <si>
+    <t>DOUBLE</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>dec</t>
+  </si>
+  <si>
+    <t>pos.eq.dec;meta.main</t>
+  </si>
+  <si>
+    <t>J2000 declination</t>
+  </si>
+  <si>
+    <t>ra_err</t>
+  </si>
+  <si>
+    <t>stat.error;pos.eq.ra</t>
+  </si>
+  <si>
+    <t>Error in Right Ascension</t>
+  </si>
+  <si>
+    <t>REAL</t>
+  </si>
+  <si>
+    <t>arcsec</t>
+  </si>
+  <si>
+    <t>dec_err</t>
+  </si>
+  <si>
+    <t>stat.error;pos.eq.dec</t>
+  </si>
+  <si>
+    <t>Error in Declination</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>em.freq</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>MHz</t>
+  </si>
+  <si>
+    <t>flux_peak</t>
+  </si>
+  <si>
+    <t>phot.flux.density;stat.max;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t>Peak flux density</t>
+  </si>
+  <si>
+    <t>mJy/beam</t>
+  </si>
+  <si>
+    <t>flux_peak_err</t>
+  </si>
+  <si>
+    <t>stat.error;phot.flux.density;stat.max;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t>Error in peak flux density</t>
+  </si>
+  <si>
+    <t>flux_int</t>
+  </si>
+  <si>
+    <t>phot.flux.density;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t>Integrated flux density</t>
+  </si>
+  <si>
+    <t>mJy</t>
+  </si>
+  <si>
+    <t>flux_int_err</t>
+  </si>
+  <si>
+    <t>stat.error;phot.flux.density;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t>Error in integrated flux density</t>
+  </si>
+  <si>
+    <t>maj_axis</t>
+  </si>
+  <si>
+    <t>phys.angSize.smajAxis;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t>FWHM major axis before deconvolution</t>
+  </si>
+  <si>
+    <t>min_axis</t>
+  </si>
+  <si>
+    <t>phys.angSize.sminAxis;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t>FWHM minor axis before deconvolution</t>
+  </si>
+  <si>
+    <t>pos_ang</t>
+  </si>
+  <si>
+    <t>phys.angSize;pos.posAng;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t>Position angle before deconvolution</t>
+  </si>
+  <si>
+    <t>maj_axis_err</t>
+  </si>
+  <si>
+    <t>stat.error;phys.angSize.smajAxis;em.radio</t>
+  </si>
+  <si>
+    <t>Error in major axis before deconvolution</t>
+  </si>
+  <si>
+    <t>min_axis_err</t>
+  </si>
+  <si>
+    <t>stat.error;phys.angSize.sminAxis;em.radio</t>
+  </si>
+  <si>
+    <t>Error in minor axis before deconvolution</t>
+  </si>
+  <si>
+    <t>pos_ang_err</t>
+  </si>
+  <si>
+    <t>stat.error;phys.angSize;pos.posAng;em.radio</t>
+  </si>
+  <si>
+    <t>Error in position angle before deconvolution</t>
+  </si>
+  <si>
+    <t>maj_axis_deconv</t>
+  </si>
+  <si>
+    <t>phys.angSize.smajAxis;em.radio;askap:meta.deconvolved</t>
+  </si>
+  <si>
+    <t>FWHM major axis after deconvolution</t>
+  </si>
+  <si>
+    <t>min_axis_deconv</t>
+  </si>
+  <si>
+    <t>phys.angSize.sminAxis;em.radio;askap:meta.deconvolved</t>
+  </si>
+  <si>
+    <t>FWHM minor axis after deconvolution</t>
+  </si>
+  <si>
+    <t>pos_ang_deconv</t>
+  </si>
+  <si>
+    <t>phys.angSize;pos.posAng;em.radio;askap:meta.deconvolved</t>
+  </si>
+  <si>
+    <t>Position angle after deconvolution</t>
+  </si>
+  <si>
+    <t>chi_squared_fit</t>
+  </si>
+  <si>
+    <t>stat.fit.chi2</t>
+  </si>
+  <si>
+    <t>Chi-squared value of Gaussian fit</t>
+  </si>
+  <si>
+    <t>rms_fit_Gauss</t>
+  </si>
+  <si>
+    <t>stat.stdev;stat.fit</t>
+  </si>
+  <si>
+    <t>RMS residual of Gaussian fit</t>
+  </si>
+  <si>
+    <t>spectral_index</t>
+  </si>
+  <si>
+    <t>spect.index;em.radio</t>
+  </si>
+  <si>
+    <t>Spectral index (First Taylor term)</t>
+  </si>
+  <si>
+    <t>spectral_curvature</t>
+  </si>
+  <si>
+    <t>askap:spect.curvature;em.radio</t>
+  </si>
+  <si>
+    <t>Spectral curvature (Second Taylor term)</t>
+  </si>
+  <si>
+    <t>rms_image</t>
+  </si>
+  <si>
+    <t>stat.stdev;phot.flux.density</t>
+  </si>
+  <si>
+    <t>rms noise level in image</t>
+  </si>
+  <si>
+    <t>has_siblings</t>
+  </si>
+  <si>
+    <t>meta.code</t>
+  </si>
+  <si>
+    <t>Source has siblings</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>fit_is_estimate</t>
+  </si>
+  <si>
+    <t>Component parameters are initial estimate, not from fit</t>
+  </si>
+  <si>
+    <t>flag_c3</t>
+  </si>
+  <si>
+    <t>Placeholder flag3</t>
+  </si>
+  <si>
+    <t>INTEGER</t>
+  </si>
+  <si>
+    <t>flag_c4</t>
+  </si>
+  <si>
+    <t>Placeholder flag4</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>meta.note</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>Column order</t>
+  </si>
+  <si>
+    <t>CASDA Field Name</t>
+  </si>
+  <si>
+    <t>Associated Selavy Name</t>
+  </si>
+  <si>
+    <t>Selavy Unit</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>ii</t>
+  </si>
+  <si>
+    <t>catalogue_id</t>
+  </si>
+  <si>
+    <t>iii</t>
+  </si>
+  <si>
+    <t>iv</t>
+  </si>
+  <si>
+    <t>project_id</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>island_id</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Columns with a selavy name of none will be left empty. They will be provided in a future Selavy verison.</t>
+  </si>
+  <si>
+    <t>degdms_cont</t>
+  </si>
+  <si>
     <t>ra_deg_cont</t>
   </si>
   <si>
-    <t>pos.eq.ra;meta.main</t>
-  </si>
-  <si>
-    <t>J2000 right ascension</t>
-  </si>
-  <si>
-    <t>DOUBLE</t>
-  </si>
-  <si>
-    <t>deg</t>
+    <t>RA</t>
   </si>
   <si>
     <t>dec_deg_cont</t>
-  </si>
-  <si>
-    <t>pos.eq.dec;meta.main</t>
-  </si>
-  <si>
-    <t>J2000 declination</t>
-  </si>
-  <si>
-    <t>ra_err</t>
-  </si>
-  <si>
-    <t>stat.error;pos.eq.ra</t>
-  </si>
-  <si>
-    <t>Error in Right Ascension</t>
-  </si>
-  <si>
-    <t>REAL</t>
-  </si>
-  <si>
-    <t>arcsec</t>
-  </si>
-  <si>
-    <t>dec_err</t>
-  </si>
-  <si>
-    <t>stat.error;pos.eq.dec</t>
-  </si>
-  <si>
-    <t>Error in Declination</t>
-  </si>
-  <si>
-    <t>freq</t>
-  </si>
-  <si>
-    <t>em.freq</t>
-  </si>
-  <si>
-    <t>Frequency</t>
-  </si>
-  <si>
-    <t>MHz</t>
-  </si>
-  <si>
-    <t>flux_peak</t>
-  </si>
-  <si>
-    <t>phot.flux.density;stat.max;em.radio;stat.fit</t>
-  </si>
-  <si>
-    <t>Peak flux density</t>
-  </si>
-  <si>
-    <t>mJy/beam</t>
-  </si>
-  <si>
-    <t>flux_peak_err</t>
-  </si>
-  <si>
-    <t>stat.error;phot.flux.density;stat.max;em.radio;stat.fit</t>
-  </si>
-  <si>
-    <t>Error in peak flux density</t>
-  </si>
-  <si>
-    <t>flux_int</t>
-  </si>
-  <si>
-    <t>phot.flux.density;em.radio;stat.fit</t>
-  </si>
-  <si>
-    <t>Integrated flux density</t>
-  </si>
-  <si>
-    <t>mJy</t>
-  </si>
-  <si>
-    <t>flux_int_err</t>
-  </si>
-  <si>
-    <t>stat.error;phot.flux.density;em.radio;stat.fit</t>
-  </si>
-  <si>
-    <t>Error in integrated flux density</t>
-  </si>
-  <si>
-    <t>maj_axis</t>
-  </si>
-  <si>
-    <t>phys.angSize.smajAxis;em.radio;stat.fit</t>
-  </si>
-  <si>
-    <t>FWHM major axis before deconvolution</t>
-  </si>
-  <si>
-    <t>min_axis</t>
-  </si>
-  <si>
-    <t>phys.angSize.sminAxis;em.radio;stat.fit</t>
-  </si>
-  <si>
-    <t>FWHM minor axis before deconvolution</t>
-  </si>
-  <si>
-    <t>pos_ang</t>
-  </si>
-  <si>
-    <t>phys.angSize;pos.posAng;em.radio;stat.fit</t>
-  </si>
-  <si>
-    <t>Position angle before deconvolution</t>
-  </si>
-  <si>
-    <t>maj_axis_err</t>
-  </si>
-  <si>
-    <t>stat.error;phys.angSize.smajAxis;em.radio</t>
-  </si>
-  <si>
-    <t>Error in major axis before deconvolution</t>
-  </si>
-  <si>
-    <t>min_axis_err</t>
-  </si>
-  <si>
-    <t>stat.error;phys.angSize.sminAxis;em.radio</t>
-  </si>
-  <si>
-    <t>Error in minor axis before deconvolution</t>
-  </si>
-  <si>
-    <t>pos_ang_err</t>
-  </si>
-  <si>
-    <t>stat.error;phys.angSize;pos.posAng;em.radio</t>
-  </si>
-  <si>
-    <t>Error in position angle before deconvolution</t>
-  </si>
-  <si>
-    <t>maj_axis_deconv</t>
-  </si>
-  <si>
-    <t>phys.angSize.smajAxis;em.radio;askap:meta.deconvolved</t>
-  </si>
-  <si>
-    <t>FWHM major axis after deconvolution</t>
-  </si>
-  <si>
-    <t>min_axis_deconv</t>
-  </si>
-  <si>
-    <t>phys.angSize.sminAxis;em.radio;askap:meta.deconvolved</t>
-  </si>
-  <si>
-    <t>FWHM minor axis after deconvolution</t>
-  </si>
-  <si>
-    <t>pos_ang_deconv</t>
-  </si>
-  <si>
-    <t>phys.angSize;pos.posAng;em.radio;askap:meta.deconvolved</t>
-  </si>
-  <si>
-    <t>Position angle after deconvolution</t>
-  </si>
-  <si>
-    <t>chi_squared_fit</t>
-  </si>
-  <si>
-    <t>stat.fit.chi2</t>
-  </si>
-  <si>
-    <t>Chi-squared value of Gaussian fit</t>
-  </si>
-  <si>
-    <t>rms_fit_Gauss</t>
-  </si>
-  <si>
-    <t>stat.stdev;stat.fit</t>
-  </si>
-  <si>
-    <t>RMS residual of Gaussian fit</t>
-  </si>
-  <si>
-    <t>spectral_index</t>
-  </si>
-  <si>
-    <t>spect.index;em.radio</t>
-  </si>
-  <si>
-    <t>Spectral index (First Taylor term)</t>
-  </si>
-  <si>
-    <t>spectral_curvature</t>
-  </si>
-  <si>
-    <t>askap:spect.curvature;em.radio</t>
-  </si>
-  <si>
-    <t>Spectral curvature (Second Taylor term)</t>
-  </si>
-  <si>
-    <t>rms_image</t>
-  </si>
-  <si>
-    <t>stat.stdev;phot.flux.density</t>
-  </si>
-  <si>
-    <t>rms noise level in image</t>
-  </si>
-  <si>
-    <t>has_siblings</t>
-  </si>
-  <si>
-    <t>meta.code</t>
-  </si>
-  <si>
-    <t>Source has siblings</t>
-  </si>
-  <si>
-    <t>BOOLEAN</t>
-  </si>
-  <si>
-    <t>fit_is_estimate</t>
-  </si>
-  <si>
-    <t>Component parameters are initial estimate, not from fit</t>
-  </si>
-  <si>
-    <t>flag_c3</t>
-  </si>
-  <si>
-    <t>Placeholder flag3</t>
-  </si>
-  <si>
-    <t>INTEGER</t>
-  </si>
-  <si>
-    <t>flag_c4</t>
-  </si>
-  <si>
-    <t>Placeholder flag4</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>meta.note</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>TEXT</t>
-  </si>
-  <si>
-    <t>Column order</t>
-  </si>
-  <si>
-    <t>CASDA Field Name</t>
-  </si>
-  <si>
-    <t>Associated Selavy Name</t>
-  </si>
-  <si>
-    <t>Selavy Unit</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>ii</t>
-  </si>
-  <si>
-    <t>catalogue_id</t>
-  </si>
-  <si>
-    <t>iii</t>
-  </si>
-  <si>
-    <t>iv</t>
-  </si>
-  <si>
-    <t>project_id</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>island_id</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Columns with a selavy name of none will be left empty. They will be provided in a future Selavy verison.</t>
-  </si>
-  <si>
-    <t>degdms_cont</t>
-  </si>
-  <si>
-    <t>RA</t>
   </si>
   <si>
     <t>DEC</t>
@@ -869,7 +875,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -958,7 +964,7 @@
   <dimension ref="1:37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
@@ -7313,7 +7319,7 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
         <v>38</v>
       </c>
@@ -8357,7 +8363,7 @@
       <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
         <v>43</v>
       </c>
@@ -12412,10 +12418,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>38</v>
+        <v>148</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>42</v>
@@ -12427,10 +12433,10 @@
         <v>6</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>43</v>
+        <v>150</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D15" s="25" t="s">
         <v>42</v>
@@ -12442,7 +12448,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>136</v>
@@ -12455,7 +12461,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>136</v>
@@ -12471,10 +12477,10 @@
         <v>58</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E18" s="16"/>
     </row>
@@ -12499,10 +12505,10 @@
         <v>65</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E20" s="16"/>
     </row>
@@ -12527,7 +12533,7 @@
         <v>72</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>50</v>
@@ -12542,7 +12548,7 @@
         <v>75</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D23" s="25" t="s">
         <v>50</v>
@@ -12557,7 +12563,7 @@
         <v>78</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D24" s="25" t="s">
         <v>42</v>
@@ -12572,7 +12578,7 @@
         <v>90</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>50</v>
@@ -12587,7 +12593,7 @@
         <v>93</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D26" s="25" t="s">
         <v>50</v>
@@ -12602,7 +12608,7 @@
         <v>96</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>42</v>
@@ -12617,7 +12623,7 @@
         <v>99</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D28" s="25" t="s">
         <v>136</v>
@@ -12632,7 +12638,7 @@
         <v>102</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>61</v>
@@ -12673,10 +12679,10 @@
         <v>111</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E32" s="16"/>
     </row>
@@ -12685,7 +12691,7 @@
         <v>24</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C33" s="25" t="s">
         <v>136</v>
@@ -12698,7 +12704,7 @@
         <v>25</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C34" s="25" t="s">
         <v>136</v>
@@ -12786,62 +12792,62 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D41" s="28" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D42" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D43" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D44" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D45" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D46" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D47" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D48" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D49" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D50" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D51" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D52" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ASKAPSDP-2344 Updating slice generation to honour the lsm_view flag in the spreadsheets. Now only fields that have lsm_view=1 are written into the DTO files. Now I just need to generate a data marshalling function for transferring from the ORM classes to the DTO
</commit_message>
<xml_diff>
--- a/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
+++ b/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="180">
   <si>
     <t>gsm.continuum_component 
 10 November 2016</t>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>BIGINT</t>
-  </si>
-  <si>
-    <t>Including in the LSM view for testing, but it is not actually required</t>
   </si>
   <si>
     <t>sb_id</t>
@@ -875,7 +872,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -964,7 +961,7 @@
   <dimension ref="1:37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
@@ -3086,7 +3083,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="2" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
         <v>16</v>
       </c>
@@ -3108,19 +3105,17 @@
         <v>0</v>
       </c>
       <c r="I4" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>19</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>18</v>
@@ -3143,16 +3138,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>24</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>25</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="15" t="n">
@@ -4185,16 +4180,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="C7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>28</v>
-      </c>
       <c r="D7" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="15" t="n">
@@ -4210,7 +4205,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K7" s="0"/>
       <c r="L7" s="0"/>
@@ -5229,19 +5224,19 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="C8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="D8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>33</v>
       </c>
       <c r="F8" s="15" t="n">
         <v>0</v>
@@ -5256,7 +5251,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K8" s="0"/>
       <c r="L8" s="0"/>
@@ -6275,19 +6270,19 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="C9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="D9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>37</v>
       </c>
       <c r="F9" s="15" t="n">
         <v>0</v>
@@ -6302,7 +6297,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K9" s="0"/>
       <c r="L9" s="0"/>
@@ -7321,19 +7316,19 @@
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="C10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="D10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="E10" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>42</v>
       </c>
       <c r="F10" s="15" t="n">
         <v>1</v>
@@ -8365,19 +8360,19 @@
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="C11" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>45</v>
-      </c>
       <c r="D11" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>42</v>
       </c>
       <c r="F11" s="15" t="n">
         <v>1</v>
@@ -9409,19 +9404,19 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="C12" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="D12" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="E12" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="F12" s="15" t="n">
         <v>1</v>
@@ -10453,19 +10448,19 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="C13" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>53</v>
-      </c>
       <c r="D13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="F13" s="15" t="n">
         <v>1</v>
@@ -11497,19 +11492,19 @@
     </row>
     <row r="14" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="C14" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="D14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="F14" s="15" t="n">
         <v>1</v>
@@ -11527,19 +11522,19 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="C15" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="D15" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>60</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>61</v>
       </c>
       <c r="F15" s="15" t="n">
         <v>1</v>
@@ -11557,19 +11552,19 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="C16" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>64</v>
-      </c>
       <c r="D16" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F16" s="15" t="n">
         <v>1</v>
@@ -11587,19 +11582,19 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="C17" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="D17" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>67</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>68</v>
       </c>
       <c r="F17" s="15" t="n">
         <v>1</v>
@@ -11617,19 +11612,19 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="C18" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>71</v>
-      </c>
       <c r="D18" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F18" s="15" t="n">
         <v>1</v>
@@ -11647,19 +11642,19 @@
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="C19" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>74</v>
-      </c>
       <c r="D19" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="F19" s="15" t="n">
         <v>1</v>
@@ -11677,19 +11672,19 @@
     </row>
     <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="C20" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>77</v>
-      </c>
       <c r="D20" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="F20" s="15" t="n">
         <v>1</v>
@@ -11707,19 +11702,19 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="C21" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>80</v>
-      </c>
       <c r="D21" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="15" t="n">
         <v>1</v>
@@ -11737,19 +11732,19 @@
     </row>
     <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="C22" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>83</v>
-      </c>
       <c r="D22" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="F22" s="15" t="n">
         <v>1</v>
@@ -11767,19 +11762,19 @@
     </row>
     <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="C23" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>86</v>
-      </c>
       <c r="D23" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="F23" s="15" t="n">
         <v>1</v>
@@ -11797,19 +11792,19 @@
     </row>
     <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="C24" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>89</v>
-      </c>
       <c r="D24" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24" s="15" t="n">
         <v>1</v>
@@ -11827,19 +11822,19 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="C25" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>92</v>
-      </c>
       <c r="D25" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="F25" s="15" t="n">
         <v>1</v>
@@ -11857,19 +11852,19 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="C26" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>95</v>
-      </c>
       <c r="D26" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="F26" s="15" t="n">
         <v>1</v>
@@ -11887,19 +11882,19 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="C27" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>98</v>
-      </c>
       <c r="D27" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F27" s="15" t="n">
         <v>1</v>
@@ -11917,16 +11912,16 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="C28" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="14" t="s">
-        <v>101</v>
-      </c>
       <c r="D28" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="15" t="n">
@@ -11945,19 +11940,19 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="C29" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="14" t="s">
-        <v>104</v>
-      </c>
       <c r="D29" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F29" s="15" t="n">
         <v>1</v>
@@ -11975,16 +11970,16 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>107</v>
-      </c>
       <c r="D30" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="15" t="n">
@@ -12003,16 +11998,16 @@
     </row>
     <row r="31" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="C31" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="14" t="s">
-        <v>110</v>
-      </c>
       <c r="D31" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="15" t="n">
@@ -12031,19 +12026,19 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="C32" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>113</v>
-      </c>
       <c r="D32" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F32" s="15" t="n">
         <v>1</v>
@@ -12061,16 +12056,16 @@
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="C33" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="D33" s="14" t="s">
         <v>116</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>117</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="15" t="n">
@@ -12089,16 +12084,16 @@
     </row>
     <row r="34" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B34" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>119</v>
-      </c>
       <c r="D34" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="15" t="n">
@@ -12117,16 +12112,16 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B35" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C35" s="14" t="s">
+      <c r="D35" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>122</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="15" t="n">
@@ -12145,16 +12140,16 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B36" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>124</v>
-      </c>
       <c r="D36" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="15" t="n">
@@ -12173,16 +12168,16 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="C37" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="D37" s="14" t="s">
         <v>127</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>128</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="15" t="n">
@@ -12251,19 +12246,19 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="D2" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="E2" s="23" t="s">
         <v>132</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12275,76 +12270,76 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="C4" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>136</v>
-      </c>
       <c r="D4" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>138</v>
-      </c>
       <c r="C5" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>141</v>
-      </c>
       <c r="C7" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>143</v>
-      </c>
       <c r="C8" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E8" s="16"/>
     </row>
@@ -12360,13 +12355,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E10" s="16"/>
     </row>
@@ -12375,13 +12370,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E11" s="16"/>
     </row>
@@ -12390,14 +12385,14 @@
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12405,10 +12400,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="16"/>
@@ -12418,13 +12413,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="C14" s="25" t="s">
-        <v>149</v>
-      </c>
       <c r="D14" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="16"/>
     </row>
@@ -12433,13 +12428,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>151</v>
-      </c>
       <c r="D15" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="16"/>
     </row>
@@ -12448,10 +12443,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="16"/>
@@ -12461,10 +12456,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="16"/>
@@ -12474,13 +12469,13 @@
         <v>9</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>154</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>155</v>
       </c>
       <c r="E18" s="16"/>
     </row>
@@ -12489,10 +12484,10 @@
         <v>10</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="16"/>
@@ -12502,13 +12497,13 @@
         <v>11</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="D20" s="25" t="s">
         <v>156</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>157</v>
       </c>
       <c r="E20" s="16"/>
     </row>
@@ -12517,10 +12512,10 @@
         <v>12</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="16"/>
@@ -12530,13 +12525,13 @@
         <v>13</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" s="16"/>
     </row>
@@ -12545,13 +12540,13 @@
         <v>14</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="16"/>
     </row>
@@ -12560,13 +12555,13 @@
         <v>15</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E24" s="16"/>
     </row>
@@ -12575,13 +12570,13 @@
         <v>16</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E25" s="16"/>
     </row>
@@ -12590,13 +12585,13 @@
         <v>17</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E26" s="16"/>
     </row>
@@ -12605,13 +12600,13 @@
         <v>18</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E27" s="16"/>
     </row>
@@ -12620,13 +12615,13 @@
         <v>19</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E28" s="16"/>
     </row>
@@ -12635,13 +12630,13 @@
         <v>20</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" s="16"/>
     </row>
@@ -12650,10 +12645,10 @@
         <v>21</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="16"/>
@@ -12663,10 +12658,10 @@
         <v>22</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="16"/>
@@ -12676,13 +12671,13 @@
         <v>23</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E32" s="16"/>
     </row>
@@ -12691,10 +12686,10 @@
         <v>24</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D33" s="25"/>
       <c r="E33" s="16"/>
@@ -12704,10 +12699,10 @@
         <v>25</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="16"/>
@@ -12717,10 +12712,10 @@
         <v>26</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="16"/>
@@ -12730,10 +12725,10 @@
         <v>27</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="16"/>
@@ -12743,10 +12738,10 @@
         <v>28</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="16"/>
@@ -12756,10 +12751,10 @@
         <v>29</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="16"/>
@@ -12769,10 +12764,10 @@
         <v>30</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D39" s="25"/>
       <c r="E39" s="16"/>
@@ -12782,72 +12777,72 @@
         <v>31</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="16"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D41" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D42" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D43" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D44" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D45" s="0" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D46" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D47" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D48" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D49" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D50" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D51" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D52" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ASKAPSDP-2526 Code generation of ORM->Ice data marshalling function is complete. Initial functional tests passing but still need to add some more
</commit_message>
<xml_diff>
--- a/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
+++ b/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
@@ -872,7 +872,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -961,7 +961,7 @@
   <dimension ref="1:37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
@@ -3136,7 +3136,7 @@
       <c r="J5" s="14"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
         <v>21</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="14"/>
       <c r="K6" s="19"/>

</xml_diff>

<commit_message>
ASKAPSDP-2572 adding new code generation flags for the search criteria API to the other spreadsheets
</commit_message>
<xml_diff>
--- a/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
+++ b/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda.continuum_component_description.xlsx
@@ -873,64 +873,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="9" tint="0.59996337778862885"/>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="9" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="9" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1341,7 +1289,7 @@
   <dimension ref="A1:AMM37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12803,12 +12751,12 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:K499">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:K1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>